<commit_message>
Copying column in case of modification is now working
</commit_message>
<xml_diff>
--- a/test/data/test_src.xlsx
+++ b/test/data/test_src.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="56">
   <si>
     <t xml:space="preserve">Activity</t>
   </si>
@@ -65,6 +65,12 @@
   </si>
   <si>
     <t xml:space="preserve">Vehicle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arrival</t>
+  </si>
+  <si>
+    <t xml:space="preserve">departure</t>
   </si>
   <si>
     <t xml:space="preserve">Activ</t>
@@ -188,9 +194,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yy"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -258,7 +265,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -269,6 +276,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -288,13 +299,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O1048576"/>
+  <dimension ref="A1:Q18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L5" activeCellId="0" sqref="L5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="10.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.06"/>
@@ -304,7 +315,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="17.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="24.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="23.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="23.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="21.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="10.51"/>
   </cols>
@@ -355,240 +366,263 @@
       <c r="O1" s="0" t="s">
         <v>14</v>
       </c>
+      <c r="P1" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="0" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F2" s="1" t="n">
         <v>25923</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
+      </c>
+      <c r="P2" s="3" t="n">
+        <v>36526</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F3" s="1" t="n">
         <v>25924</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
+      </c>
+      <c r="P3" s="3" t="n">
+        <v>40210</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F4" s="1" t="n">
         <v>29493</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
+      </c>
+      <c r="Q4" s="3" t="n">
+        <v>43597</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F5" s="1" t="n">
         <v>31341</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
+      </c>
+      <c r="P5" s="3" t="n">
+        <v>40909</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F6" s="1" t="n">
         <v>32891</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="M6" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
+      </c>
+      <c r="Q6" s="3" t="n">
+        <v>43597</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F7" s="1" t="n">
         <v>29273</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="M7" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
+      </c>
+      <c r="Q7" s="3" t="n">
+        <v>43597</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>